<commit_message>
MFG losses calculation progress
created files to support mfg eff calcs, structured the journal, starte working on the first section.
</commit_message>
<xml_diff>
--- a/PV_DEMICE/baselines/SupportingMaterial/2020-10-baselineDev-Si_mfg_eff.xlsx
+++ b/PV_DEMICE/baselines/SupportingMaterial/2020-10-baselineDev-Si_mfg_eff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blond\Documents\NREL\CE4PV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blond\Documents\GitHub\CircularEconomy-MassFlowCalculator\PV_DEMICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D155141-5F43-48C2-BAFB-13703DA7A6FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B7D318-BED0-44BB-B2F1-C86EE0B2DF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="21600" windowHeight="11040" xr2:uid="{FFB4C077-1C71-4E42-8327-656C3ABB9F64}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FFB4C077-1C71-4E42-8327-656C3ABB9F64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
   <si>
     <t>Kerf losses &amp; Total Thickness Variation</t>
   </si>
@@ -128,29 +128,35 @@
     <t>g extra for crucible and squaring</t>
   </si>
   <si>
-    <t>g/wafer, incl. non-kerf loss</t>
-  </si>
-  <si>
     <t>*assumes 10g/wafer</t>
   </si>
   <si>
     <t>AVG, only includes kerf</t>
   </si>
   <si>
-    <t>Si_gpercell</t>
-  </si>
-  <si>
-    <t>cm cell side</t>
-  </si>
-  <si>
-    <t>cm^2</t>
+    <t>Si g/wafer each year</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Si_gpercell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year             </t>
+  </si>
+  <si>
+    <t>(%)</t>
+  </si>
+  <si>
+    <t>MFG eff</t>
+  </si>
+  <si>
+    <t>g/wafer, incl. other losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +192,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +216,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -243,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -254,13 +279,14 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,88 +601,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53123EC1-FE23-4789-843A-B1965AD73125}">
-  <dimension ref="A1:AE64"/>
+  <dimension ref="A1:Z64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="U33" sqref="U33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="13" customWidth="1"/>
-    <col min="15" max="15" width="10" style="13" customWidth="1"/>
-    <col min="16" max="16" width="4.140625" customWidth="1"/>
-    <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="20" width="4.140625" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" customWidth="1"/>
-    <col min="22" max="22" width="22.5703125" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="13"/>
+    <col min="3" max="3" width="12.81640625" customWidth="1"/>
+    <col min="4" max="5" width="4.7265625" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" customWidth="1"/>
+    <col min="8" max="8" width="3.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9" style="12" customWidth="1"/>
+    <col min="18" max="18" width="10" style="12" customWidth="1"/>
+    <col min="19" max="20" width="4.1796875" customWidth="1"/>
+    <col min="21" max="21" width="19.453125" customWidth="1"/>
+    <col min="22" max="22" width="22.54296875" customWidth="1"/>
+    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="L1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>34</v>
+      <c r="O1" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="U1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:31">
-      <c r="E2" t="s">
+    <row r="2" spans="1:26">
+      <c r="I2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="Q2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="R2" s="9" t="s">
         <v>29</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -665,42 +695,46 @@
       <c r="V2" t="s">
         <v>18</v>
       </c>
-      <c r="AE2">
-        <v>2.3290000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="E3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="M3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="5"/>
-      <c r="N3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="9"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" s="8"/>
       <c r="U3" t="s">
         <v>11</v>
       </c>
@@ -719,750 +753,816 @@
       <c r="Z3" t="s">
         <v>6</v>
       </c>
-      <c r="AB3">
-        <v>156</v>
-      </c>
-      <c r="AC3">
-        <f>AB3^2</f>
-        <v>24336</v>
-      </c>
-      <c r="AD3">
-        <f>0.0364*2.4336</f>
-        <v>8.8583040000000016E-2</v>
-      </c>
-      <c r="AE3">
-        <f>AD3*AE2</f>
-        <v>0.20630990016000006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>1990</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="13">
+        <v>50</v>
+      </c>
+      <c r="C4">
         <v>400</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="3">
         <v>0.04</v>
       </c>
-      <c r="AB4">
-        <f>156/10</f>
-        <v>15.6</v>
-      </c>
-      <c r="AC4">
-        <f>AB4^2</f>
-        <v>243.35999999999999</v>
-      </c>
-      <c r="AD4">
-        <f>0.018*AB4^2</f>
-        <v>4.3804799999999995</v>
-      </c>
-      <c r="AE4">
-        <f>AD4*AE2</f>
-        <v>10.20213792</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31">
+      <c r="E4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>1991</v>
       </c>
-      <c r="B5">
-        <f>C5*10000</f>
+      <c r="B5" s="13">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <f>D5*10000</f>
         <v>392.86</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>3.9286000000000001E-2</v>
       </c>
-      <c r="AB5" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>1992</v>
       </c>
-      <c r="B6">
-        <f t="shared" ref="B6:B23" si="0">C6*10000</f>
+      <c r="B6" s="13">
+        <v>50</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C23" si="0">D6*10000</f>
         <v>385.71000000000004</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D6" s="3">
         <v>3.8571000000000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:31">
+      <c r="E6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>1993</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="13">
+        <v>50</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>378.57</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>3.7857000000000002E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:31">
+      <c r="E7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>1994</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="13">
+        <v>50</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>371.43</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="3">
         <v>3.7143000000000002E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:31">
+      <c r="E8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>1995</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
+        <v>50</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>364.29</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="3">
         <v>3.6429000000000003E-2</v>
       </c>
-      <c r="E9">
-        <f>0.5*B9</f>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>1995</v>
+      </c>
+      <c r="G9" s="3">
+        <v>13.256584999999999</v>
+      </c>
+      <c r="I9">
+        <f>0.5*C9</f>
         <v>182.14500000000001</v>
       </c>
-      <c r="G9" t="s">
+      <c r="K9" t="s">
         <v>7</v>
       </c>
-      <c r="Q9">
-        <v>0.20647199999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31">
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>1996</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
+        <v>50</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>357.14000000000004</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="3">
         <v>3.5714000000000003E-2</v>
       </c>
-      <c r="Q10">
-        <v>0.20242299999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>1996</v>
+      </c>
+      <c r="G10" s="3">
+        <v>14.057179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>1997</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="13">
+        <v>50</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>350.00000000000006</v>
       </c>
-      <c r="C11" s="3">
+      <c r="D11" s="3">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="Q11">
-        <v>0.198375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>1997</v>
+      </c>
+      <c r="G11" s="3">
+        <v>14.856109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>1998</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
+        <v>50</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>342.85999999999996</v>
       </c>
-      <c r="C12" s="3">
+      <c r="D12" s="3">
         <v>3.4285999999999997E-2</v>
       </c>
-      <c r="Q12">
-        <v>0.194326</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>1998</v>
+      </c>
+      <c r="G12" s="3">
+        <v>15.650880000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>1999</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="13">
+        <v>50</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>335.71</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="3">
         <v>3.3570999999999997E-2</v>
       </c>
-      <c r="Q13">
-        <v>0.190278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>1999</v>
+      </c>
+      <c r="G13" s="3">
+        <v>16.438997000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>2000</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="13">
+        <v>50</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>328.57</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <v>3.2856999999999997E-2</v>
       </c>
-      <c r="Q14">
-        <v>0.18623000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>2000</v>
+      </c>
+      <c r="G14" s="3">
+        <v>17.217963999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>2001</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="13">
+        <v>50</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>321.43</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <v>3.2142999999999998E-2</v>
       </c>
-      <c r="Q15">
-        <v>0.18218100000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>2001</v>
+      </c>
+      <c r="G15" s="3">
+        <v>16.978679</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>2002</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="13">
+        <v>50</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>314.28999999999996</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <v>3.1428999999999999E-2</v>
       </c>
-      <c r="Q16">
-        <v>0.17813300000000001</v>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>2002</v>
+      </c>
+      <c r="G16" s="3">
+        <v>16.733920999999999</v>
       </c>
     </row>
     <row r="17" spans="1:26">
       <c r="A17">
         <v>2003</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="13">
+        <v>50</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
         <v>307.14000000000004</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <v>3.0714000000000002E-2</v>
       </c>
-      <c r="E17">
-        <f>0.5*B17</f>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
+        <v>2003</v>
+      </c>
+      <c r="G17" s="3">
+        <v>16.483653</v>
+      </c>
+      <c r="I17">
+        <f>0.5*C17</f>
         <v>153.57000000000002</v>
       </c>
-      <c r="G17" t="s">
+      <c r="K17" t="s">
         <v>7</v>
-      </c>
-      <c r="Q17">
-        <v>0.17408399999999999</v>
       </c>
     </row>
     <row r="18" spans="1:26">
       <c r="A18">
         <v>2004</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>300</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <v>0.03</v>
       </c>
-      <c r="Q18">
-        <v>0.17003599999999999</v>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>2004</v>
+      </c>
+      <c r="G18" s="3">
+        <v>16.227838999999999</v>
       </c>
     </row>
     <row r="19" spans="1:26">
       <c r="A19">
         <v>2005</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="Q19">
-        <v>0.14169599999999999</v>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3">
+        <v>2005</v>
+      </c>
+      <c r="G19" s="3">
+        <v>13.62989</v>
       </c>
     </row>
     <row r="20" spans="1:26">
       <c r="A20">
         <v>2006</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>200</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <v>0.02</v>
       </c>
-      <c r="Q20">
-        <v>0.113357</v>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>2006</v>
+      </c>
+      <c r="G20" s="3">
+        <v>10.989601</v>
       </c>
     </row>
     <row r="21" spans="1:26">
       <c r="A21">
         <v>2007</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <v>1.9E-2</v>
       </c>
-      <c r="Q21">
-        <v>0.10768900000000001</v>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>2007</v>
+      </c>
+      <c r="G21" s="3">
+        <v>10.521843000000001</v>
       </c>
     </row>
     <row r="22" spans="1:26">
       <c r="A22">
         <v>2008</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>180</v>
       </c>
-      <c r="C22" s="3">
+      <c r="D22" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="Q22">
-        <v>0.102021</v>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <v>2008</v>
+      </c>
+      <c r="G22" s="3">
+        <v>10.045786</v>
       </c>
     </row>
     <row r="23" spans="1:26">
       <c r="A23">
         <v>2009</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="Q23">
-        <v>0.102021</v>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <v>2009</v>
+      </c>
+      <c r="G23" s="3">
+        <v>10.123811</v>
       </c>
     </row>
     <row r="24" spans="1:26">
       <c r="A24">
         <v>2010</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>180</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>2010</v>
+      </c>
+      <c r="G24" s="3">
+        <v>10.202138</v>
+      </c>
+      <c r="I24">
         <v>155</v>
       </c>
-      <c r="H24" s="12">
-        <f>(B24+E24)/B24*100</f>
-        <v>186.11111111111111</v>
-      </c>
-      <c r="I24" s="12">
-        <f>10*H24/100</f>
-        <v>18.611111111111111</v>
-      </c>
-      <c r="J24" s="5">
-        <f t="shared" ref="J24:J30" si="1">($B24+E24)/$B24*100</f>
-        <v>186.11111111111111</v>
-      </c>
-      <c r="K24" s="5">
-        <f t="shared" ref="K24:K30" si="2">($B24+F24)/$B24*100</f>
-        <v>100</v>
-      </c>
-      <c r="L24" s="6">
-        <f t="shared" ref="L24:L30" si="3">10*J24/100</f>
-        <v>18.611111111111111</v>
-      </c>
-      <c r="M24" s="6">
-        <f t="shared" ref="M24:M30" si="4">10*K24/100</f>
-        <v>10</v>
-      </c>
-      <c r="N24" s="9">
-        <f>L24+$L$32</f>
-        <v>20.791666666666668</v>
-      </c>
-      <c r="O24" s="9">
-        <f>M24+$M$32</f>
-        <v>11.50277777777778</v>
-      </c>
-      <c r="Q24">
-        <v>0.102021</v>
-      </c>
+      <c r="L24" s="11">
+        <f>((C24/(C24+I24)))*100</f>
+        <v>53.731343283582092</v>
+      </c>
+      <c r="M24" s="5">
+        <f>$C24/($C24+I24)*100</f>
+        <v>53.731343283582092</v>
+      </c>
+      <c r="N24" s="5"/>
+      <c r="O24" s="6">
+        <f>10*(1+M24/100)</f>
+        <v>15.373134328358208</v>
+      </c>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="8">
+        <f>O24+$O$32</f>
+        <v>18.596494984095912</v>
+      </c>
+      <c r="R24" s="8"/>
     </row>
     <row r="25" spans="1:26">
       <c r="A25">
         <v>2011</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>180</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>2011</v>
+      </c>
+      <c r="G25" s="3">
+        <v>10.202138</v>
+      </c>
+      <c r="I25">
         <v>152</v>
       </c>
-      <c r="F25">
+      <c r="J25">
         <v>148</v>
       </c>
-      <c r="H25" s="12">
-        <f>(AVERAGE(E25:F25)+B25)/B25*100</f>
-        <v>183.33333333333331</v>
-      </c>
-      <c r="I25" s="12">
-        <f t="shared" ref="I25:I31" si="5">10*H25/100</f>
-        <v>18.333333333333329</v>
-      </c>
-      <c r="J25" s="5">
-        <f t="shared" si="1"/>
-        <v>184.44444444444446</v>
-      </c>
-      <c r="K25" s="5">
-        <f t="shared" si="2"/>
-        <v>182.22222222222223</v>
-      </c>
-      <c r="L25" s="6">
-        <f t="shared" si="3"/>
-        <v>18.444444444444446</v>
-      </c>
-      <c r="M25" s="6">
-        <f t="shared" si="4"/>
-        <v>18.222222222222221</v>
-      </c>
-      <c r="N25" s="9">
-        <f t="shared" ref="N25:N30" si="6">L25+$L$32</f>
-        <v>20.625000000000004</v>
-      </c>
-      <c r="O25" s="9">
-        <f t="shared" ref="O25:O31" si="7">M25+$M$32</f>
-        <v>19.725000000000001</v>
-      </c>
-      <c r="Q25">
-        <v>0.102021</v>
+      <c r="L25" s="11">
+        <f t="shared" ref="L25:L31" si="1">((C25/(C25+I25)))*100</f>
+        <v>54.216867469879517</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" ref="M25:M31" si="2">$C25/($C25+I25)*100</f>
+        <v>54.216867469879517</v>
+      </c>
+      <c r="N25" s="5">
+        <f>$C25/($C25+J25)*100</f>
+        <v>54.878048780487809</v>
+      </c>
+      <c r="O25" s="6">
+        <f t="shared" ref="O25:P33" si="3">10*(1+M25/100)</f>
+        <v>15.421686746987952</v>
+      </c>
+      <c r="P25" s="6">
+        <f>10*(1+N25/100)</f>
+        <v>15.487804878048781</v>
+      </c>
+      <c r="Q25" s="8">
+        <f t="shared" ref="Q25:Q30" si="4">O25+$O$32</f>
+        <v>18.645047402725659</v>
+      </c>
+      <c r="R25" s="8">
+        <f t="shared" ref="R25:R32" si="5">P25+$P$32</f>
+        <v>14.920352047860103</v>
       </c>
     </row>
     <row r="26" spans="1:26">
       <c r="A26">
         <v>2012</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>180</v>
       </c>
-      <c r="C26" s="3">
+      <c r="D26" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>2012</v>
+      </c>
+      <c r="G26" s="3">
+        <v>10.202138</v>
+      </c>
+      <c r="I26">
         <v>160</v>
       </c>
-      <c r="F26">
+      <c r="J26">
         <v>155</v>
       </c>
-      <c r="H26" s="12">
-        <f t="shared" ref="H26:H31" si="8">(AVERAGE(E26:F26)+B26)/B26*100</f>
-        <v>187.5</v>
-      </c>
-      <c r="I26" s="12">
+      <c r="L26" s="11">
+        <f t="shared" si="1"/>
+        <v>52.941176470588239</v>
+      </c>
+      <c r="M26" s="5">
+        <f t="shared" si="2"/>
+        <v>52.941176470588239</v>
+      </c>
+      <c r="N26" s="5">
+        <f>$C26/($C26+J26)*100</f>
+        <v>53.731343283582092</v>
+      </c>
+      <c r="O26" s="6">
+        <f t="shared" si="3"/>
+        <v>15.294117647058822</v>
+      </c>
+      <c r="P26" s="6">
+        <f t="shared" si="3"/>
+        <v>15.373134328358208</v>
+      </c>
+      <c r="Q26" s="8">
+        <f t="shared" si="4"/>
+        <v>18.517478302796526</v>
+      </c>
+      <c r="R26" s="8">
         <f t="shared" si="5"/>
-        <v>18.75</v>
-      </c>
-      <c r="J26" s="5">
-        <f t="shared" si="1"/>
-        <v>188.88888888888889</v>
-      </c>
-      <c r="K26" s="5">
-        <f t="shared" si="2"/>
-        <v>186.11111111111111</v>
-      </c>
-      <c r="L26" s="6">
-        <f t="shared" si="3"/>
-        <v>18.888888888888889</v>
-      </c>
-      <c r="M26" s="6">
-        <f t="shared" si="4"/>
-        <v>18.611111111111111</v>
-      </c>
-      <c r="N26" s="9">
-        <f t="shared" si="6"/>
-        <v>21.069444444444446</v>
-      </c>
-      <c r="O26" s="9">
-        <f t="shared" si="7"/>
-        <v>20.113888888888891</v>
-      </c>
-      <c r="Q26">
-        <v>0.102021</v>
+        <v>14.80568149816953</v>
       </c>
     </row>
     <row r="27" spans="1:26">
       <c r="A27">
         <v>2013</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>180</v>
       </c>
-      <c r="C27" s="3">
+      <c r="D27" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
+        <v>2013</v>
+      </c>
+      <c r="G27" s="3">
+        <v>10.202138</v>
+      </c>
+      <c r="I27">
         <v>150</v>
       </c>
-      <c r="F27">
+      <c r="J27">
         <v>138</v>
       </c>
-      <c r="H27" s="12">
-        <f t="shared" si="8"/>
-        <v>180</v>
-      </c>
-      <c r="I27" s="12">
+      <c r="L27" s="11">
+        <f t="shared" si="1"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="M27" s="5">
+        <f t="shared" si="2"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="N27" s="5">
+        <f>$C27/($C27+J27)*100</f>
+        <v>56.60377358490566</v>
+      </c>
+      <c r="O27" s="6">
+        <f t="shared" si="3"/>
+        <v>15.454545454545453</v>
+      </c>
+      <c r="P27" s="6">
+        <f t="shared" si="3"/>
+        <v>15.660377358490564</v>
+      </c>
+      <c r="Q27" s="8">
+        <f t="shared" si="4"/>
+        <v>18.677906110283161</v>
+      </c>
+      <c r="R27" s="8">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="J27" s="5">
-        <f t="shared" si="1"/>
-        <v>183.33333333333331</v>
-      </c>
-      <c r="K27" s="5">
-        <f t="shared" si="2"/>
-        <v>176.66666666666666</v>
-      </c>
-      <c r="L27" s="6">
-        <f t="shared" si="3"/>
-        <v>18.333333333333329</v>
-      </c>
-      <c r="M27" s="6">
-        <f t="shared" si="4"/>
-        <v>17.666666666666664</v>
-      </c>
-      <c r="N27" s="9">
-        <f t="shared" si="6"/>
-        <v>20.513888888888886</v>
-      </c>
-      <c r="O27" s="9">
-        <f t="shared" si="7"/>
-        <v>19.169444444444444</v>
-      </c>
-      <c r="Q27">
-        <v>0.102021</v>
+        <v>15.092924528301886</v>
       </c>
     </row>
     <row r="28" spans="1:26">
       <c r="A28">
         <v>2014</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>180</v>
       </c>
-      <c r="C28" s="3">
+      <c r="D28" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>2014</v>
+      </c>
+      <c r="G28" s="3">
+        <v>10.202138</v>
+      </c>
+      <c r="I28">
         <v>150</v>
       </c>
-      <c r="F28">
+      <c r="J28">
         <v>130</v>
       </c>
-      <c r="H28" s="12">
-        <f t="shared" si="8"/>
-        <v>177.77777777777777</v>
-      </c>
-      <c r="I28" s="12">
+      <c r="L28" s="11">
+        <f t="shared" si="1"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="M28" s="5">
+        <f t="shared" si="2"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="N28" s="5">
+        <f>$C28/($C28+J28)*100</f>
+        <v>58.064516129032263</v>
+      </c>
+      <c r="O28" s="6">
+        <f t="shared" si="3"/>
+        <v>15.454545454545453</v>
+      </c>
+      <c r="P28" s="6">
+        <f t="shared" si="3"/>
+        <v>15.806451612903224</v>
+      </c>
+      <c r="Q28" s="8">
+        <f t="shared" si="4"/>
+        <v>18.677906110283161</v>
+      </c>
+      <c r="R28" s="8">
         <f t="shared" si="5"/>
-        <v>17.777777777777779</v>
-      </c>
-      <c r="J28" s="5">
-        <f t="shared" si="1"/>
-        <v>183.33333333333331</v>
-      </c>
-      <c r="K28" s="5">
-        <f t="shared" si="2"/>
-        <v>172.22222222222223</v>
-      </c>
-      <c r="L28" s="6">
-        <f t="shared" si="3"/>
-        <v>18.333333333333329</v>
-      </c>
-      <c r="M28" s="6">
-        <f t="shared" si="4"/>
-        <v>17.222222222222221</v>
-      </c>
-      <c r="N28" s="9">
-        <f t="shared" si="6"/>
-        <v>20.513888888888886</v>
-      </c>
-      <c r="O28" s="9">
-        <f t="shared" si="7"/>
-        <v>18.725000000000001</v>
-      </c>
-      <c r="Q28">
-        <v>0.102021</v>
+        <v>15.238998782714546</v>
       </c>
     </row>
     <row r="29" spans="1:26">
       <c r="A29">
         <v>2015</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>180</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>2015</v>
+      </c>
+      <c r="G29" s="3">
+        <v>10.202138</v>
+      </c>
+      <c r="I29">
         <v>150</v>
       </c>
-      <c r="F29">
+      <c r="J29">
         <v>125</v>
       </c>
-      <c r="H29" s="12">
-        <f t="shared" si="8"/>
-        <v>176.38888888888889</v>
-      </c>
-      <c r="I29" s="12">
+      <c r="L29" s="11">
+        <f t="shared" si="1"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="M29" s="5">
+        <f t="shared" si="2"/>
+        <v>54.54545454545454</v>
+      </c>
+      <c r="N29" s="5">
+        <f>$C29/($C29+J29)*100</f>
+        <v>59.016393442622949</v>
+      </c>
+      <c r="O29" s="6">
+        <f t="shared" si="3"/>
+        <v>15.454545454545453</v>
+      </c>
+      <c r="P29" s="6">
+        <f t="shared" si="3"/>
+        <v>15.901639344262295</v>
+      </c>
+      <c r="Q29" s="8">
+        <f t="shared" si="4"/>
+        <v>18.677906110283161</v>
+      </c>
+      <c r="R29" s="8">
         <f t="shared" si="5"/>
-        <v>17.638888888888889</v>
-      </c>
-      <c r="J29" s="5">
-        <f t="shared" si="1"/>
-        <v>183.33333333333331</v>
-      </c>
-      <c r="K29" s="5">
-        <f t="shared" si="2"/>
-        <v>169.44444444444443</v>
-      </c>
-      <c r="L29" s="6">
-        <f t="shared" si="3"/>
-        <v>18.333333333333329</v>
-      </c>
-      <c r="M29" s="6">
-        <f t="shared" si="4"/>
-        <v>16.944444444444443</v>
-      </c>
-      <c r="N29" s="9">
-        <f t="shared" si="6"/>
-        <v>20.513888888888886</v>
-      </c>
-      <c r="O29" s="9">
-        <f t="shared" si="7"/>
-        <v>18.447222222222223</v>
-      </c>
-      <c r="Q29">
-        <v>0.102021</v>
+        <v>15.334186514073616</v>
       </c>
     </row>
     <row r="30" spans="1:26">
       <c r="A30">
         <v>2016</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>180</v>
       </c>
-      <c r="C30" s="3">
+      <c r="D30" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G30" s="3">
+        <v>10.225484</v>
+      </c>
+      <c r="I30">
         <v>135</v>
       </c>
-      <c r="F30">
+      <c r="J30">
         <v>110</v>
       </c>
-      <c r="H30" s="12">
-        <f t="shared" si="8"/>
-        <v>168.05555555555557</v>
-      </c>
-      <c r="I30" s="12">
+      <c r="L30" s="11">
+        <f t="shared" si="1"/>
+        <v>57.142857142857139</v>
+      </c>
+      <c r="M30" s="5">
+        <f t="shared" si="2"/>
+        <v>57.142857142857139</v>
+      </c>
+      <c r="N30" s="5">
+        <f>$C30/($C30+J30)*100</f>
+        <v>62.068965517241381</v>
+      </c>
+      <c r="O30" s="6">
+        <f t="shared" si="3"/>
+        <v>15.714285714285714</v>
+      </c>
+      <c r="P30" s="6">
+        <f t="shared" si="3"/>
+        <v>16.206896551724135</v>
+      </c>
+      <c r="Q30" s="8">
+        <f t="shared" si="4"/>
+        <v>18.937646370023419</v>
+      </c>
+      <c r="R30" s="8">
         <f t="shared" si="5"/>
-        <v>16.805555555555557</v>
-      </c>
-      <c r="J30" s="5">
-        <f t="shared" si="1"/>
-        <v>175</v>
-      </c>
-      <c r="K30" s="5">
-        <f t="shared" si="2"/>
-        <v>161.11111111111111</v>
-      </c>
-      <c r="L30" s="6">
-        <f t="shared" si="3"/>
-        <v>17.5</v>
-      </c>
-      <c r="M30" s="6">
-        <f t="shared" si="4"/>
-        <v>16.111111111111111</v>
-      </c>
-      <c r="N30" s="9">
-        <f t="shared" si="6"/>
-        <v>19.680555555555557</v>
-      </c>
-      <c r="O30" s="9">
-        <f t="shared" si="7"/>
-        <v>17.613888888888891</v>
-      </c>
-      <c r="Q30">
-        <v>0.102255</v>
+        <v>15.639443721535457</v>
       </c>
     </row>
     <row r="31" spans="1:26">
       <c r="A31">
         <v>2017</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>180</v>
       </c>
-      <c r="C31" s="3">
+      <c r="D31" s="3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3">
+        <v>2017</v>
+      </c>
+      <c r="G31" s="3">
+        <v>10.277241</v>
+      </c>
+      <c r="I31">
         <v>125</v>
       </c>
-      <c r="F31">
+      <c r="J31">
         <v>85</v>
       </c>
-      <c r="H31" s="12">
-        <f t="shared" si="8"/>
-        <v>158.33333333333331</v>
-      </c>
-      <c r="I31" s="12">
+      <c r="L31" s="11">
+        <f t="shared" si="1"/>
+        <v>59.016393442622949</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" si="2"/>
+        <v>59.016393442622949</v>
+      </c>
+      <c r="N31" s="5">
+        <f>$C31/($C31+J31)*100</f>
+        <v>67.924528301886795</v>
+      </c>
+      <c r="O31" s="6">
+        <f t="shared" si="3"/>
+        <v>15.901639344262295</v>
+      </c>
+      <c r="P31" s="6">
+        <f t="shared" si="3"/>
+        <v>16.79245283018868</v>
+      </c>
+      <c r="Q31" s="8">
+        <f>O31+$O$32</f>
+        <v>19.125</v>
+      </c>
+      <c r="R31" s="8">
         <f t="shared" si="5"/>
-        <v>15.83333333333333</v>
-      </c>
-      <c r="J31" s="5">
-        <f>($B31+E31)/$B31*100</f>
-        <v>169.44444444444443</v>
-      </c>
-      <c r="K31" s="5">
-        <f>($B31+F31)/$B31*100</f>
-        <v>147.22222222222223</v>
-      </c>
-      <c r="L31" s="6">
-        <f>10*J31/100</f>
-        <v>16.944444444444443</v>
-      </c>
-      <c r="M31" s="6">
-        <f>10*K31/100</f>
-        <v>14.722222222222221</v>
-      </c>
-      <c r="N31" s="9">
-        <f>L31+$L$32</f>
-        <v>19.125</v>
-      </c>
-      <c r="O31" s="9">
-        <f t="shared" si="7"/>
         <v>16.225000000000001</v>
-      </c>
-      <c r="Q31">
-        <v>0.102772</v>
       </c>
       <c r="U31">
         <v>16.75</v>
@@ -1487,28 +1587,32 @@
       <c r="A32">
         <v>2018</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>176.40833330000001</v>
       </c>
-      <c r="C32" s="3">
+      <c r="D32" s="3">
         <v>1.7641E-2</v>
       </c>
-      <c r="K32" s="5"/>
-      <c r="L32" s="7">
-        <f>AVERAGE(W31:X31)-L31</f>
-        <v>2.1805555555555571</v>
-      </c>
-      <c r="M32" s="7">
-        <f>AVERAGE(U31:V31)-M31</f>
-        <v>1.50277777777778</v>
-      </c>
-      <c r="N32" s="13" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>2018</v>
+      </c>
+      <c r="G32" s="3">
+        <v>10.097915</v>
+      </c>
+      <c r="N32" s="5"/>
+      <c r="O32" s="7">
+        <f>AVERAGE(W31:X31)-O31</f>
+        <v>3.2233606557377055</v>
+      </c>
+      <c r="P32" s="7">
+        <f>AVERAGE(U31:V31)-P31</f>
+        <v>-0.56745283018867809</v>
+      </c>
+      <c r="Q32" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="O32" s="9"/>
-      <c r="Q32">
-        <v>0.100979</v>
-      </c>
+      <c r="R32" s="8"/>
       <c r="U32">
         <v>16.5</v>
       </c>
@@ -1526,36 +1630,40 @@
       <c r="A33">
         <v>2019</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>172.66666670000001</v>
       </c>
-      <c r="C33" s="3">
+      <c r="D33" s="3">
         <v>1.7267000000000001E-2</v>
       </c>
-      <c r="F33">
+      <c r="E33" s="3"/>
+      <c r="F33" s="3">
+        <v>2019</v>
+      </c>
+      <c r="G33" s="3">
+        <v>9.9873150000000006</v>
+      </c>
+      <c r="J33">
         <v>75</v>
       </c>
-      <c r="K33" s="5">
-        <f>($B33+F33)/$B33*100</f>
-        <v>143.43629342790805</v>
-      </c>
-      <c r="L33" s="5"/>
-      <c r="M33" s="6">
-        <f>10*K33/100</f>
-        <v>14.343629342790805</v>
-      </c>
-      <c r="N33" s="9"/>
-      <c r="O33" s="14">
-        <f>M33+$M$32</f>
-        <v>15.846407120568585</v>
-      </c>
-      <c r="Q33">
-        <v>9.9873000000000003E-2</v>
+      <c r="N33" s="5">
+        <f>$C33/($C33+J33)*100</f>
+        <v>69.717362049836154</v>
+      </c>
+      <c r="O33" s="5"/>
+      <c r="P33" s="6">
+        <f>10*(1+N33/100)</f>
+        <v>16.971736204983614</v>
+      </c>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="14">
+        <f>P33+$P$32</f>
+        <v>16.404283374794936</v>
       </c>
       <c r="U33">
         <v>16</v>
       </c>
-      <c r="V33" s="8">
+      <c r="V33" s="15">
         <v>15</v>
       </c>
       <c r="Y33" t="s">
@@ -1569,23 +1677,27 @@
       <c r="A34" s="1">
         <v>2020</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="13"/>
+      <c r="C34" s="1">
         <v>163.18333329999999</v>
       </c>
-      <c r="C34" s="3">
+      <c r="D34" s="3">
         <v>1.6317999999999999E-2</v>
       </c>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>2020</v>
+      </c>
+      <c r="G34" s="3">
+        <v>9.7260930000000005</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="Q34">
-        <v>9.7261E-2</v>
-      </c>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
       <c r="U34" s="1">
         <v>15.2</v>
       </c>
@@ -1603,25 +1715,33 @@
       <c r="A35">
         <v>2021</v>
       </c>
-      <c r="C35" s="3">
+      <c r="D35" s="3">
         <v>1.5774E-2</v>
       </c>
-      <c r="Q35">
-        <v>9.5107999999999998E-2</v>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <v>2021</v>
+      </c>
+      <c r="G35" s="3">
+        <v>9.5108490000000003</v>
       </c>
     </row>
     <row r="36" spans="1:26">
       <c r="A36">
         <v>2022</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>152.30000000000001</v>
       </c>
-      <c r="C36" s="3">
+      <c r="D36" s="3">
         <v>1.523E-2</v>
       </c>
-      <c r="Q36">
-        <v>9.2871999999999996E-2</v>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>2022</v>
+      </c>
+      <c r="G36" s="3">
+        <v>9.2872140000000005</v>
       </c>
       <c r="U36">
         <v>15</v>
@@ -1640,25 +1760,33 @@
       <c r="A37">
         <v>2023</v>
       </c>
-      <c r="C37" s="3">
+      <c r="D37" s="3">
         <v>1.4963000000000001E-2</v>
       </c>
-      <c r="Q37">
-        <v>9.1366000000000003E-2</v>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3">
+        <v>2023</v>
+      </c>
+      <c r="G37" s="3">
+        <v>9.1365789999999993</v>
       </c>
     </row>
     <row r="38" spans="1:26">
       <c r="A38">
         <v>2024</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>146.96666669999999</v>
       </c>
-      <c r="C38" s="3">
+      <c r="D38" s="3">
         <v>1.4697E-2</v>
       </c>
-      <c r="Q38">
-        <v>9.0246000000000007E-2</v>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>2024</v>
+      </c>
+      <c r="G38" s="3">
+        <v>9.0245840000000008</v>
       </c>
       <c r="U38">
         <v>14</v>
@@ -1677,36 +1805,48 @@
       <c r="A39">
         <v>2025</v>
       </c>
-      <c r="C39" s="3">
+      <c r="D39" s="3">
         <v>1.4427000000000001E-2</v>
       </c>
-      <c r="Q39">
-        <v>8.9851E-2</v>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3">
+        <v>2025</v>
+      </c>
+      <c r="G39" s="3">
+        <v>8.9851390000000002</v>
       </c>
     </row>
     <row r="40" spans="1:26">
       <c r="A40">
         <v>2026</v>
       </c>
-      <c r="C40" s="3">
+      <c r="D40" s="3">
         <v>1.4158E-2</v>
       </c>
-      <c r="Q40" s="1">
-        <v>8.9257000000000003E-2</v>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3">
+        <v>2026</v>
+      </c>
+      <c r="G40" s="3">
+        <v>8.9256890000000002</v>
       </c>
     </row>
     <row r="41" spans="1:26">
       <c r="A41">
         <v>2027</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>138.88499999999999</v>
       </c>
-      <c r="C41" s="3">
+      <c r="D41" s="3">
         <v>1.3887999999999999E-2</v>
       </c>
-      <c r="Q41">
-        <v>8.8468000000000005E-2</v>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3">
+        <v>2027</v>
+      </c>
+      <c r="G41" s="3">
+        <v>8.846819</v>
       </c>
       <c r="U41">
         <v>13.8</v>
@@ -1725,39 +1865,51 @@
       <c r="A42">
         <v>2028</v>
       </c>
-      <c r="C42" s="3">
+      <c r="D42" s="3">
         <v>1.3757E-2</v>
       </c>
-      <c r="Q42">
-        <v>8.7763999999999995E-2</v>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3">
+        <v>2028</v>
+      </c>
+      <c r="G42" s="3">
+        <v>8.7763799999999996</v>
       </c>
     </row>
     <row r="43" spans="1:26">
       <c r="A43">
         <v>2029</v>
       </c>
-      <c r="C43" s="3">
+      <c r="D43" s="3">
         <v>1.3625999999999999E-2</v>
       </c>
-      <c r="Q43">
-        <v>8.7057999999999996E-2</v>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3">
+        <v>2029</v>
+      </c>
+      <c r="G43" s="3">
+        <v>8.7057699999999993</v>
       </c>
     </row>
     <row r="44" spans="1:26">
       <c r="A44">
         <v>2030</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>134.94999999999999</v>
       </c>
-      <c r="C44" s="3">
+      <c r="D44" s="3">
         <v>1.3495E-2</v>
       </c>
-      <c r="F44">
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
+        <v>2030</v>
+      </c>
+      <c r="G44" s="3">
+        <v>8.6349889999999991</v>
+      </c>
+      <c r="J44">
         <v>50</v>
-      </c>
-      <c r="Q44">
-        <v>8.6349999999999996E-2</v>
       </c>
       <c r="U44">
         <v>13</v>

</xml_diff>

<commit_message>
Further dev on MFG eff of Si
Working on the 2017 kerf as proxy check.
</commit_message>
<xml_diff>
--- a/PV_DEMICE/baselines/SupportingMaterial/2020-10-baselineDev-Si_mfg_eff.xlsx
+++ b/PV_DEMICE/baselines/SupportingMaterial/2020-10-baselineDev-Si_mfg_eff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blond\Documents\GitHub\CircularEconomy-MassFlowCalculator\PV_DEMICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B7D318-BED0-44BB-B2F1-C86EE0B2DF8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F13E465-6F1B-4C00-B6E7-4EEBF9184B49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{FFB4C077-1C71-4E42-8327-656C3ABB9F64}"/>
+    <workbookView xWindow="780" yWindow="840" windowWidth="14400" windowHeight="7365" xr2:uid="{FFB4C077-1C71-4E42-8327-656C3ABB9F64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -604,35 +604,35 @@
   <dimension ref="A1:Z64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="L14" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U33" sqref="U33"/>
+      <selection pane="bottomRight" activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.7265625" style="13"/>
-    <col min="3" max="3" width="12.81640625" customWidth="1"/>
-    <col min="4" max="5" width="4.7265625" customWidth="1"/>
-    <col min="6" max="6" width="7.54296875" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" customWidth="1"/>
-    <col min="8" max="8" width="3.7265625" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="13"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="12" customWidth="1"/>
     <col min="18" max="18" width="10" style="12" customWidth="1"/>
-    <col min="19" max="20" width="4.1796875" customWidth="1"/>
-    <col min="21" max="21" width="19.453125" customWidth="1"/>
-    <col min="22" max="22" width="22.54296875" customWidth="1"/>
-    <col min="23" max="23" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="4.140625" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" customWidth="1"/>
+    <col min="22" max="22" width="22.5703125" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1233,11 +1233,11 @@
         <v>54.216867469879517</v>
       </c>
       <c r="N25" s="5">
-        <f>$C25/($C25+J25)*100</f>
+        <f t="shared" ref="N25:N31" si="3">$C25/($C25+J25)*100</f>
         <v>54.878048780487809</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" ref="O25:P33" si="3">10*(1+M25/100)</f>
+        <f t="shared" ref="O25:P31" si="4">10*(1+M25/100)</f>
         <v>15.421686746987952</v>
       </c>
       <c r="P25" s="6">
@@ -1245,11 +1245,11 @@
         <v>15.487804878048781</v>
       </c>
       <c r="Q25" s="8">
-        <f t="shared" ref="Q25:Q30" si="4">O25+$O$32</f>
+        <f t="shared" ref="Q25:Q30" si="5">O25+$O$32</f>
         <v>18.645047402725659</v>
       </c>
       <c r="R25" s="8">
-        <f t="shared" ref="R25:R32" si="5">P25+$P$32</f>
+        <f t="shared" ref="R25:R31" si="6">P25+$P$32</f>
         <v>14.920352047860103</v>
       </c>
     </row>
@@ -1285,23 +1285,23 @@
         <v>52.941176470588239</v>
       </c>
       <c r="N26" s="5">
-        <f>$C26/($C26+J26)*100</f>
+        <f t="shared" si="3"/>
         <v>53.731343283582092</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.294117647058822</v>
       </c>
       <c r="P26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.373134328358208</v>
       </c>
       <c r="Q26" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.517478302796526</v>
       </c>
       <c r="R26" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14.80568149816953</v>
       </c>
     </row>
@@ -1337,23 +1337,23 @@
         <v>54.54545454545454</v>
       </c>
       <c r="N27" s="5">
-        <f>$C27/($C27+J27)*100</f>
+        <f t="shared" si="3"/>
         <v>56.60377358490566</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.454545454545453</v>
       </c>
       <c r="P27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.660377358490564</v>
       </c>
       <c r="Q27" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.677906110283161</v>
       </c>
       <c r="R27" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.092924528301886</v>
       </c>
     </row>
@@ -1389,23 +1389,23 @@
         <v>54.54545454545454</v>
       </c>
       <c r="N28" s="5">
-        <f>$C28/($C28+J28)*100</f>
+        <f t="shared" si="3"/>
         <v>58.064516129032263</v>
       </c>
       <c r="O28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.454545454545453</v>
       </c>
       <c r="P28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.806451612903224</v>
       </c>
       <c r="Q28" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.677906110283161</v>
       </c>
       <c r="R28" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.238998782714546</v>
       </c>
     </row>
@@ -1441,23 +1441,23 @@
         <v>54.54545454545454</v>
       </c>
       <c r="N29" s="5">
-        <f>$C29/($C29+J29)*100</f>
+        <f t="shared" si="3"/>
         <v>59.016393442622949</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.454545454545453</v>
       </c>
       <c r="P29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.901639344262295</v>
       </c>
       <c r="Q29" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.677906110283161</v>
       </c>
       <c r="R29" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.334186514073616</v>
       </c>
     </row>
@@ -1493,23 +1493,23 @@
         <v>57.142857142857139</v>
       </c>
       <c r="N30" s="5">
-        <f>$C30/($C30+J30)*100</f>
+        <f t="shared" si="3"/>
         <v>62.068965517241381</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.714285714285714</v>
       </c>
       <c r="P30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.206896551724135</v>
       </c>
       <c r="Q30" s="8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.937646370023419</v>
       </c>
       <c r="R30" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15.639443721535457</v>
       </c>
     </row>
@@ -1545,15 +1545,15 @@
         <v>59.016393442622949</v>
       </c>
       <c r="N31" s="5">
-        <f>$C31/($C31+J31)*100</f>
+        <f t="shared" si="3"/>
         <v>67.924528301886795</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.901639344262295</v>
       </c>
       <c r="P31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.79245283018868</v>
       </c>
       <c r="Q31" s="8">
@@ -1561,7 +1561,7 @@
         <v>19.125</v>
       </c>
       <c r="R31" s="8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.225000000000001</v>
       </c>
       <c r="U31">

</xml_diff>